<commit_message>
create test case for valid credentials
</commit_message>
<xml_diff>
--- a/test_scenarios.xlsx
+++ b/test_scenarios.xlsx
@@ -4,7 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Info" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Sign-Up" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Registration" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Login" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="Order assigne" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="45">
   <si>
     <t>Project Name</t>
   </si>
   <si>
+    <t>Facebook Application</t>
+  </si>
+  <si>
     <t>Designed By</t>
+  </si>
+  <si>
+    <t>Joshua</t>
   </si>
   <si>
     <t>Android Versions</t>
@@ -53,13 +61,22 @@
     <t>Web</t>
   </si>
   <si>
+    <t>Web Notes</t>
+  </si>
+  <si>
     <t>Prereq.</t>
+  </si>
+  <si>
+    <t>- User should have open the facebook registration page on their browser</t>
+  </si>
+  <si>
+    <t>Register with valid credentials [using phone number]</t>
   </si>
   <si>
     <t>1.1</t>
   </si>
   <si>
-    <t>Fail</t>
+    <t>Enter a valid firstname</t>
   </si>
   <si>
     <t>Ready to Test</t>
@@ -68,7 +85,31 @@
     <t>1.2</t>
   </si>
   <si>
+    <t>Enter a vaild surname</t>
+  </si>
+  <si>
     <t>1.3</t>
+  </si>
+  <si>
+    <t>Enter a valid phone number</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>Enter a valid password (min 8 legth, at least one capital letter)</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Enter a valid DOB (Should not be less than 18 years)</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>Enter a valid gender</t>
   </si>
   <si>
     <t>2.1</t>
@@ -102,6 +143,12 @@
   </si>
   <si>
     <t>5.1</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -339,6 +386,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -365,30 +420,34 @@
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="8"/>
@@ -418,6 +477,1456 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="6.38"/>
+    <col customWidth="1" min="2" max="2" width="50.75"/>
+    <col customWidth="1" min="3" max="3" width="47.13"/>
+    <col customWidth="1" min="4" max="4" width="14.25"/>
+    <col customWidth="1" min="5" max="5" width="29.0"/>
+    <col customWidth="1" min="6" max="6" width="14.25"/>
+    <col customWidth="1" min="7" max="9" width="29.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="17"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="17"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="21"/>
+      <c r="H24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="22"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="13"/>
+      <c r="B28" s="22"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="15"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="15"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="15"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="15"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="15"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="15"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="15"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="15"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="15"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="15"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="15"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="15"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="15"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="15"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="15"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="13"/>
+      <c r="B48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="15"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="15"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="15"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="15"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="13"/>
+      <c r="B53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="15"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="15"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="15"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="15"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="15"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="13"/>
+      <c r="B59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="15"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="15"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="15"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="15"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="15"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="13"/>
+      <c r="B65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="15"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="15"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="15"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="15"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="15"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="15"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="15"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="15"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="15"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="13"/>
+      <c r="B75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="15"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="15"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="15"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="15"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="15"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="15"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="21"/>
+      <c r="H81" s="21"/>
+      <c r="I81" s="21"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="15"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="15"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="15"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="15"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="13"/>
+      <c r="B86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="15"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+      <c r="I87" s="18"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="15"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="15"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="15"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="15"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="15"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="13"/>
+      <c r="B93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="15"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="15"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="15"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="21"/>
+      <c r="I96" s="21"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="13"/>
+      <c r="B97" s="14"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="21"/>
+      <c r="H97" s="21"/>
+      <c r="I97" s="21"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="15"/>
+      <c r="B98" s="16"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="21"/>
+      <c r="I98" s="21"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="15"/>
+      <c r="B99" s="19"/>
+      <c r="C99" s="19"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="21"/>
+      <c r="H99" s="21"/>
+      <c r="I99" s="21"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="15"/>
+      <c r="B100" s="19"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="21"/>
+      <c r="I100" s="21"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="15"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="21"/>
+      <c r="H101" s="21"/>
+      <c r="I101" s="21"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="15"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="21"/>
+      <c r="H102" s="21"/>
+      <c r="I102" s="21"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="15"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="19"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+      <c r="I103" s="21"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="15"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="21"/>
+      <c r="H104" s="21"/>
+      <c r="I104" s="21"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="15"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="21"/>
+      <c r="H105" s="21"/>
+      <c r="I105" s="21"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="15"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="16"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="21"/>
+      <c r="H106" s="21"/>
+      <c r="I106" s="21"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="15"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="24"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="21"/>
+      <c r="H107" s="21"/>
+      <c r="I107" s="21"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="15"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="19"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="21"/>
+      <c r="H108" s="21"/>
+      <c r="I108" s="21"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="15"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="17"/>
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+      <c r="I109" s="21"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="15"/>
+      <c r="B110" s="19"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="25"/>
+      <c r="F110" s="17"/>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+      <c r="I110" s="21"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="15"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="17"/>
+      <c r="G111" s="21"/>
+      <c r="H111" s="21"/>
+      <c r="I111" s="21"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="15"/>
+      <c r="B112" s="19"/>
+      <c r="C112" s="19"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="25"/>
+      <c r="F112" s="17"/>
+      <c r="G112" s="21"/>
+      <c r="H112" s="21"/>
+      <c r="I112" s="21"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="15"/>
+      <c r="B113" s="19"/>
+      <c r="C113" s="19"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="24"/>
+      <c r="F113" s="17"/>
+      <c r="G113" s="21"/>
+      <c r="H113" s="21"/>
+      <c r="I113" s="21"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="15"/>
+      <c r="B114" s="19"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="25"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="21"/>
+      <c r="H114" s="21"/>
+      <c r="I114" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B18:D18"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D4:D9 F4:F9 H4:I9 D11:D13 F11:F13 H11:I13 D15:D17 F15:F17 H15:I17 D19:D22 F19:F22 H19:I22 D24 F24 H24:I24 D26:D27 F26:F27 D29:D30 F29:F30 D32:D39 F32:F39 D41:D47 F41:F47 D49:D52 F49:F52 D54:D58 F54:F58 D60:D64 F60:F64 D66:D74 F66:F74 D76:D85 F76:F85 D87:D92 F87:F92 D94:D96 F94:F114 D98:D114">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH(("Pass"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D9 F4:F9 H4:I9 D11:D13 F11:F13 H11:I13 D15:D17 F15:F17 H15:I17 D19:D22 F19:F22 H19:I22 D24 F24 H24:I24 D26:D27 F26:F27 D29:D30 F29:F30 D32:D39 F32:F39 D41:D47 F41:F47 D49:D52 F49:F52 D54:D58 F54:F58 D60:D64 F60:F64 D66:D74 F66:F74 D76:D85 F76:F85 D87:D92 F87:F92 D94:D96 F94:F114 D98:D114">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH(("Fail"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D9 F4:F9 H4:I9 D11:D13 F11:F13 H11:I13 D15:D17 F15:F17 H15:I17 D19:D22 F19:F22 H19:I22 D24 F24 H24:I24 D26:D27 F26:F27 D29:D30 F29:F30 D32:D39 F32:F39 D41:D47 F41:F47 D49:D52 F49:F52 D54:D58 F54:F58 D60:D64 F60:F64 D66:D74 F66:F74 D76:D85 F76:F85 D87:D92 F87:F92 D94:D96 F94:F114 D98:D114">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Block / Skip">
+      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D9 F4:F9 H4:I9 D11:D13 F11:F13 H11:I13 D15:D17 F15:F17 H15:I17 D19:D22 F19:F22 H19:I22 D24 F24 H24:I24 D26:D27 F26:F27 D29:D30 F29:F30 D32:D39 F32:F39 D41:D47 F41:F47 D49:D52 F49:F52 D54:D58 F54:F58 D60:D64 F60:F64 D66:D74 F66:F74 D76:D85 F76:F85 D87:D92 F87:F92 D94:D96 F94:F96 D98:D114 F98:F114">
+      <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <tabColor rgb="FFF1C232"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="6.38"/>
     <col customWidth="1" min="2" max="2" width="43.88"/>
     <col customWidth="1" min="3" max="3" width="47.13"/>
     <col customWidth="1" min="4" max="4" width="14.25"/>
@@ -428,33 +1937,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -478,56 +1987,56 @@
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="15" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="15" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
@@ -542,56 +2051,56 @@
     </row>
     <row r="8">
       <c r="A8" s="15" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="16"/>
       <c r="D8" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="15" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="16"/>
       <c r="D9" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G9" s="18"/>
       <c r="H9" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="15" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="16"/>
       <c r="D10" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -606,56 +2115,56 @@
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="16"/>
       <c r="D12" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="15" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="15" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="16"/>
       <c r="D14" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
@@ -670,74 +2179,74 @@
     </row>
     <row r="16">
       <c r="A16" s="15" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G16" s="18"/>
       <c r="H16" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="15" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="15" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="16"/>
       <c r="D18" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="15" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
       <c r="D19" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20">
@@ -754,20 +2263,20 @@
     </row>
     <row r="21">
       <c r="A21" s="15" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G21" s="21"/>
       <c r="H21" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
@@ -1649,7 +3158,1288 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B45:D45"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F111 D95:D111">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH(("Pass"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F111 D95:D111">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH(("Fail"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F111 D95:D111">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Block / Skip">
+      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F93 D95:D111 F95:F111">
+      <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <tabColor rgb="FFF1C232"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="6.38"/>
+    <col customWidth="1" min="2" max="2" width="43.88"/>
+    <col customWidth="1" min="3" max="3" width="47.13"/>
+    <col customWidth="1" min="4" max="4" width="14.25"/>
+    <col customWidth="1" min="5" max="5" width="29.0"/>
+    <col customWidth="1" min="6" max="6" width="14.25"/>
+    <col customWidth="1" min="7" max="8" width="29.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="13"/>
+      <c r="B22" s="22"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="22"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="15"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="15"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="15"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="15"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="15"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="15"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="15"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="15"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="15"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="15"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="15"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="15"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="15"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="15"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="15"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="15"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="15"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="15"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="13"/>
+      <c r="B50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="15"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="15"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="15"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="15"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="15"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="15"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="15"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="15"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="15"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="15"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="13"/>
+      <c r="B62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="15"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="15"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="15"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="15"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="15"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="15"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="15"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="15"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="13"/>
+      <c r="B72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="15"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="15"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="15"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="15"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="15"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="15"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="21"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="15"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="15"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="15"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="15"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="13"/>
+      <c r="B83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="15"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="15"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="15"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="15"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="15"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="15"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="13"/>
+      <c r="B90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="15"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="15"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="15"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="21"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="13"/>
+      <c r="B94" s="14"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="21"/>
+      <c r="H94" s="21"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="15"/>
+      <c r="B95" s="16"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="21"/>
+      <c r="H95" s="21"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="15"/>
+      <c r="B96" s="19"/>
+      <c r="C96" s="19"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="21"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="15"/>
+      <c r="B97" s="19"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="17"/>
+      <c r="G97" s="21"/>
+      <c r="H97" s="21"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="15"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="21"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="15"/>
+      <c r="B99" s="19"/>
+      <c r="C99" s="16"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="21"/>
+      <c r="H99" s="21"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="15"/>
+      <c r="B100" s="19"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="21"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="15"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="21"/>
+      <c r="H101" s="21"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="15"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="21"/>
+      <c r="H102" s="21"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="15"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="16"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="15"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="21"/>
+      <c r="H104" s="21"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="15"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="21"/>
+      <c r="H105" s="21"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="15"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="19"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="21"/>
+      <c r="H106" s="21"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="15"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="21"/>
+      <c r="H107" s="21"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="15"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="19"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="21"/>
+      <c r="H108" s="21"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="15"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="25"/>
+      <c r="F109" s="17"/>
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="15"/>
+      <c r="B110" s="19"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="24"/>
+      <c r="F110" s="17"/>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="15"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="17"/>
+      <c r="G111" s="21"/>
+      <c r="H111" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="B72:D72"/>
@@ -1662,6 +4452,7 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B50:D50"/>
     <mergeCell ref="B45:D45"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F111 D95:D111">

</xml_diff>

<commit_message>
create test case for valid credentials (#3)
</commit_message>
<xml_diff>
--- a/test_scenarios.xlsx
+++ b/test_scenarios.xlsx
@@ -4,7 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Info" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Sign-Up" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Registration" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Login" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="Order assigne" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="45">
   <si>
     <t>Project Name</t>
   </si>
   <si>
+    <t>Facebook Application</t>
+  </si>
+  <si>
     <t>Designed By</t>
+  </si>
+  <si>
+    <t>Joshua</t>
   </si>
   <si>
     <t>Android Versions</t>
@@ -53,13 +61,22 @@
     <t>Web</t>
   </si>
   <si>
+    <t>Web Notes</t>
+  </si>
+  <si>
     <t>Prereq.</t>
+  </si>
+  <si>
+    <t>- User should have open the facebook registration page on their browser</t>
+  </si>
+  <si>
+    <t>Register with valid credentials [using phone number]</t>
   </si>
   <si>
     <t>1.1</t>
   </si>
   <si>
-    <t>Fail</t>
+    <t>Enter a valid firstname</t>
   </si>
   <si>
     <t>Ready to Test</t>
@@ -68,7 +85,31 @@
     <t>1.2</t>
   </si>
   <si>
+    <t>Enter a vaild surname</t>
+  </si>
+  <si>
     <t>1.3</t>
+  </si>
+  <si>
+    <t>Enter a valid phone number</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>Enter a valid password (min 8 legth, at least one capital letter)</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Enter a valid DOB (Should not be less than 18 years)</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>Enter a valid gender</t>
   </si>
   <si>
     <t>2.1</t>
@@ -102,6 +143,12 @@
   </si>
   <si>
     <t>5.1</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -339,6 +386,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -365,30 +420,34 @@
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="8"/>
@@ -418,6 +477,1456 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="6.38"/>
+    <col customWidth="1" min="2" max="2" width="50.75"/>
+    <col customWidth="1" min="3" max="3" width="47.13"/>
+    <col customWidth="1" min="4" max="4" width="14.25"/>
+    <col customWidth="1" min="5" max="5" width="29.0"/>
+    <col customWidth="1" min="6" max="6" width="14.25"/>
+    <col customWidth="1" min="7" max="9" width="29.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="17"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="17"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="21"/>
+      <c r="H24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="22"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="13"/>
+      <c r="B28" s="22"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="15"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="15"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="15"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="15"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="15"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="15"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="15"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="15"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="15"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="15"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="15"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="15"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="15"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="15"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="15"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="13"/>
+      <c r="B48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="15"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="15"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="15"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="15"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="13"/>
+      <c r="B53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="15"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="15"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="15"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="15"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="15"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="13"/>
+      <c r="B59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="15"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="15"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="15"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="15"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="15"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="13"/>
+      <c r="B65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="15"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="15"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="15"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="15"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="15"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="15"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="15"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="15"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="15"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="13"/>
+      <c r="B75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="15"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="15"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="15"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="15"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="15"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="15"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="21"/>
+      <c r="H81" s="21"/>
+      <c r="I81" s="21"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="15"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="15"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="15"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="15"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="13"/>
+      <c r="B86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="15"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+      <c r="I87" s="18"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="15"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="15"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="15"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="15"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="15"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="13"/>
+      <c r="B93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="15"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="15"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="15"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="21"/>
+      <c r="I96" s="21"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="13"/>
+      <c r="B97" s="14"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="21"/>
+      <c r="H97" s="21"/>
+      <c r="I97" s="21"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="15"/>
+      <c r="B98" s="16"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="21"/>
+      <c r="I98" s="21"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="15"/>
+      <c r="B99" s="19"/>
+      <c r="C99" s="19"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="21"/>
+      <c r="H99" s="21"/>
+      <c r="I99" s="21"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="15"/>
+      <c r="B100" s="19"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="21"/>
+      <c r="I100" s="21"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="15"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="21"/>
+      <c r="H101" s="21"/>
+      <c r="I101" s="21"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="15"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="21"/>
+      <c r="H102" s="21"/>
+      <c r="I102" s="21"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="15"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="19"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+      <c r="I103" s="21"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="15"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="21"/>
+      <c r="H104" s="21"/>
+      <c r="I104" s="21"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="15"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="21"/>
+      <c r="H105" s="21"/>
+      <c r="I105" s="21"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="15"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="16"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="21"/>
+      <c r="H106" s="21"/>
+      <c r="I106" s="21"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="15"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="24"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="21"/>
+      <c r="H107" s="21"/>
+      <c r="I107" s="21"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="15"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="19"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="21"/>
+      <c r="H108" s="21"/>
+      <c r="I108" s="21"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="15"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="17"/>
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+      <c r="I109" s="21"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="15"/>
+      <c r="B110" s="19"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="25"/>
+      <c r="F110" s="17"/>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+      <c r="I110" s="21"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="15"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="17"/>
+      <c r="G111" s="21"/>
+      <c r="H111" s="21"/>
+      <c r="I111" s="21"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="15"/>
+      <c r="B112" s="19"/>
+      <c r="C112" s="19"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="25"/>
+      <c r="F112" s="17"/>
+      <c r="G112" s="21"/>
+      <c r="H112" s="21"/>
+      <c r="I112" s="21"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="15"/>
+      <c r="B113" s="19"/>
+      <c r="C113" s="19"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="24"/>
+      <c r="F113" s="17"/>
+      <c r="G113" s="21"/>
+      <c r="H113" s="21"/>
+      <c r="I113" s="21"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="15"/>
+      <c r="B114" s="19"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="25"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="21"/>
+      <c r="H114" s="21"/>
+      <c r="I114" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B18:D18"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D4:D9 F4:F9 H4:I9 D11:D13 F11:F13 H11:I13 D15:D17 F15:F17 H15:I17 D19:D22 F19:F22 H19:I22 D24 F24 H24:I24 D26:D27 F26:F27 D29:D30 F29:F30 D32:D39 F32:F39 D41:D47 F41:F47 D49:D52 F49:F52 D54:D58 F54:F58 D60:D64 F60:F64 D66:D74 F66:F74 D76:D85 F76:F85 D87:D92 F87:F92 D94:D96 F94:F114 D98:D114">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH(("Pass"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D9 F4:F9 H4:I9 D11:D13 F11:F13 H11:I13 D15:D17 F15:F17 H15:I17 D19:D22 F19:F22 H19:I22 D24 F24 H24:I24 D26:D27 F26:F27 D29:D30 F29:F30 D32:D39 F32:F39 D41:D47 F41:F47 D49:D52 F49:F52 D54:D58 F54:F58 D60:D64 F60:F64 D66:D74 F66:F74 D76:D85 F76:F85 D87:D92 F87:F92 D94:D96 F94:F114 D98:D114">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH(("Fail"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D9 F4:F9 H4:I9 D11:D13 F11:F13 H11:I13 D15:D17 F15:F17 H15:I17 D19:D22 F19:F22 H19:I22 D24 F24 H24:I24 D26:D27 F26:F27 D29:D30 F29:F30 D32:D39 F32:F39 D41:D47 F41:F47 D49:D52 F49:F52 D54:D58 F54:F58 D60:D64 F60:F64 D66:D74 F66:F74 D76:D85 F76:F85 D87:D92 F87:F92 D94:D96 F94:F114 D98:D114">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Block / Skip">
+      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D9 F4:F9 H4:I9 D11:D13 F11:F13 H11:I13 D15:D17 F15:F17 H15:I17 D19:D22 F19:F22 H19:I22 D24 F24 H24:I24 D26:D27 F26:F27 D29:D30 F29:F30 D32:D39 F32:F39 D41:D47 F41:F47 D49:D52 F49:F52 D54:D58 F54:F58 D60:D64 F60:F64 D66:D74 F66:F74 D76:D85 F76:F85 D87:D92 F87:F92 D94:D96 F94:F96 D98:D114 F98:F114">
+      <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <tabColor rgb="FFF1C232"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="6.38"/>
     <col customWidth="1" min="2" max="2" width="43.88"/>
     <col customWidth="1" min="3" max="3" width="47.13"/>
     <col customWidth="1" min="4" max="4" width="14.25"/>
@@ -428,33 +1937,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -478,56 +1987,56 @@
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="15" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="15" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
@@ -542,56 +2051,56 @@
     </row>
     <row r="8">
       <c r="A8" s="15" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="16"/>
       <c r="D8" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="15" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="16"/>
       <c r="D9" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G9" s="18"/>
       <c r="H9" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="15" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="16"/>
       <c r="D10" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -606,56 +2115,56 @@
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="16"/>
       <c r="D12" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="15" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="15" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="16"/>
       <c r="D14" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
@@ -670,74 +2179,74 @@
     </row>
     <row r="16">
       <c r="A16" s="15" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G16" s="18"/>
       <c r="H16" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="15" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="15" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="16"/>
       <c r="D18" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="15" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
       <c r="D19" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20">
@@ -754,20 +2263,20 @@
     </row>
     <row r="21">
       <c r="A21" s="15" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G21" s="21"/>
       <c r="H21" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
@@ -1649,7 +3158,1288 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B45:D45"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F111 D95:D111">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH(("Pass"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F111 D95:D111">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH(("Fail"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F111 D95:D111">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Block / Skip">
+      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F93 D95:D111 F95:F111">
+      <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <tabColor rgb="FFF1C232"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="6.38"/>
+    <col customWidth="1" min="2" max="2" width="43.88"/>
+    <col customWidth="1" min="3" max="3" width="47.13"/>
+    <col customWidth="1" min="4" max="4" width="14.25"/>
+    <col customWidth="1" min="5" max="5" width="29.0"/>
+    <col customWidth="1" min="6" max="6" width="14.25"/>
+    <col customWidth="1" min="7" max="8" width="29.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="13"/>
+      <c r="B22" s="22"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="22"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="15"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="15"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="15"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="15"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="15"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="15"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="15"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="15"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="15"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="15"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="15"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="15"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="15"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="15"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="15"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="15"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="15"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="15"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="13"/>
+      <c r="B50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="15"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="15"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="15"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="15"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="15"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="15"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="15"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="15"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="15"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="15"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="13"/>
+      <c r="B62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="15"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="15"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="15"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="15"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="15"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="15"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="15"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="15"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="13"/>
+      <c r="B72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="15"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="15"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="15"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="15"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="15"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="15"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="21"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="15"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="15"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="15"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="15"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="13"/>
+      <c r="B83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="15"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="15"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="15"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="15"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="15"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="15"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="13"/>
+      <c r="B90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="15"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="15"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="15"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="21"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="13"/>
+      <c r="B94" s="14"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="21"/>
+      <c r="H94" s="21"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="15"/>
+      <c r="B95" s="16"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="21"/>
+      <c r="H95" s="21"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="15"/>
+      <c r="B96" s="19"/>
+      <c r="C96" s="19"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="21"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="15"/>
+      <c r="B97" s="19"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="17"/>
+      <c r="G97" s="21"/>
+      <c r="H97" s="21"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="15"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="21"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="15"/>
+      <c r="B99" s="19"/>
+      <c r="C99" s="16"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="21"/>
+      <c r="H99" s="21"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="15"/>
+      <c r="B100" s="19"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="21"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="15"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="21"/>
+      <c r="H101" s="21"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="15"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="21"/>
+      <c r="H102" s="21"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="15"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="16"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="15"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="21"/>
+      <c r="H104" s="21"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="15"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="21"/>
+      <c r="H105" s="21"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="15"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="19"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="21"/>
+      <c r="H106" s="21"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="15"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="21"/>
+      <c r="H107" s="21"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="15"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="19"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="21"/>
+      <c r="H108" s="21"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="15"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="25"/>
+      <c r="F109" s="17"/>
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="15"/>
+      <c r="B110" s="19"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="24"/>
+      <c r="F110" s="17"/>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="15"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="17"/>
+      <c r="G111" s="21"/>
+      <c r="H111" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="B72:D72"/>
@@ -1662,6 +4452,7 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B50:D50"/>
     <mergeCell ref="B45:D45"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F111 D95:D111">

</xml_diff>

<commit_message>
added valid credential test scenario
</commit_message>
<xml_diff>
--- a/test_scenarios.xlsx
+++ b/test_scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Project Name</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>user should have their browser open</t>
+  </si>
+  <si>
+    <t>Register user with valid credentials</t>
   </si>
   <si>
     <t>1.1</t>
@@ -234,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -275,6 +278,9 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="9" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1673,1047 +1679,1049 @@
       <c r="A3" s="14">
         <v>1.0</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="B3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="19"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="19"/>
+      <c r="A6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="14">
         <v>2.0</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="19"/>
+      <c r="A8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="20"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="19"/>
+      <c r="A9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="19"/>
+      <c r="A10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="14">
         <v>3.0</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="19"/>
+      <c r="A12" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="19"/>
+      <c r="A13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="19"/>
+      <c r="A14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="14">
         <v>4.0</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="19"/>
+      <c r="A16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="19"/>
+      <c r="A17" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="19"/>
+      <c r="A18" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="19"/>
+      <c r="A19" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="14">
         <v>5.0</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="19"/>
+      <c r="A21" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="14"/>
-      <c r="B22" s="22"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
+      <c r="B22" s="23"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="19"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="19"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="20"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="14"/>
-      <c r="B25" s="22"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
+      <c r="B25" s="23"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="19"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="16"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="19"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="14"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="16"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="19"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="16"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="19"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="16"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="19"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="20"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="16"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="19"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="20"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="16"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="19"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="20"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="16"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="19"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="20"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="16"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="19"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="20"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="16"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="19"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="20"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="14"/>
-      <c r="B37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
+      <c r="B37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="19"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="20"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="16"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="19"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="16"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="19"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="16"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="19"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="20"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="16"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="19"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="20"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="16"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="19"/>
+      <c r="A43" s="17"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="20"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="16"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="19"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="20"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="14"/>
-      <c r="B45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
+      <c r="B45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="16"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="19"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="20"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="16"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="19"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="20"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="16"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="19"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="20"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="16"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="19"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="20"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="14"/>
-      <c r="B50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
+      <c r="B50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="16"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="19"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="20"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="16"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="19"/>
+      <c r="A52" s="17"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="20"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="16"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="19"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="20"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="16"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="19"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="20"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="16"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="19"/>
+      <c r="A55" s="17"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="20"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="14"/>
-      <c r="B56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
+      <c r="B56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="16"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="19"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="20"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="16"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="19"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="20"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="16"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="19"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="20"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="16"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="19"/>
+      <c r="A60" s="17"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="20"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="16"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="19"/>
+      <c r="A61" s="17"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="20"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="14"/>
-      <c r="B62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
+      <c r="B62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="16"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="19"/>
+      <c r="A63" s="17"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="20"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="16"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="19"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="20"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="16"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="19"/>
+      <c r="A65" s="17"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="20"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="16"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="19"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="20"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="16"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="19"/>
+      <c r="A67" s="17"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="20"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="16"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="19"/>
+      <c r="A68" s="17"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="20"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="16"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="19"/>
+      <c r="A69" s="17"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="20"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="16"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="19"/>
+      <c r="A70" s="17"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="20"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="16"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="19"/>
+      <c r="A71" s="17"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="20"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="14"/>
-      <c r="B72" s="15"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15"/>
+      <c r="B72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="16"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="19"/>
+      <c r="A73" s="17"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="20"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="16"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="19"/>
+      <c r="A74" s="17"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="20"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="16"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="19"/>
+      <c r="A75" s="17"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="20"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="16"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="19"/>
+      <c r="A76" s="17"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="20"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="16"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="20"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="19"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="19"/>
+      <c r="A77" s="17"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="20"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="16"/>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="19"/>
+      <c r="A78" s="17"/>
+      <c r="B78" s="21"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="20"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="16"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="18"/>
-      <c r="G79" s="19"/>
+      <c r="A79" s="17"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="20"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="16"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="19"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="19"/>
+      <c r="A80" s="17"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="20"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="16"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="19"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="19"/>
+      <c r="A81" s="17"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="20"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="16"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="18"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="19"/>
+      <c r="A82" s="17"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="20"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="14"/>
-      <c r="B83" s="15"/>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="15"/>
+      <c r="B83" s="16"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="16"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="16"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="19"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="19"/>
+      <c r="A84" s="17"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="19"/>
+      <c r="G84" s="20"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="16"/>
-      <c r="B85" s="20"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="19"/>
+      <c r="A85" s="17"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="20"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="16"/>
-      <c r="B86" s="20"/>
-      <c r="C86" s="20"/>
-      <c r="D86" s="18"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="18"/>
-      <c r="G86" s="19"/>
+      <c r="A86" s="17"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="20"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="16"/>
-      <c r="B87" s="20"/>
-      <c r="C87" s="20"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="19"/>
-      <c r="F87" s="18"/>
-      <c r="G87" s="19"/>
+      <c r="A87" s="17"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="20"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="16"/>
-      <c r="B88" s="20"/>
-      <c r="C88" s="20"/>
-      <c r="D88" s="18"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="19"/>
+      <c r="A88" s="17"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="20"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="20"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="16"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="18"/>
-      <c r="G89" s="19"/>
+      <c r="A89" s="17"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="20"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="14"/>
-      <c r="B90" s="15"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="15"/>
+      <c r="B90" s="16"/>
+      <c r="E90" s="16"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="16"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="16"/>
-      <c r="B91" s="21"/>
-      <c r="C91" s="17"/>
-      <c r="D91" s="18"/>
-      <c r="E91" s="19"/>
-      <c r="F91" s="18"/>
-      <c r="G91" s="19"/>
+      <c r="A91" s="17"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="20"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="16"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="17"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="19"/>
-      <c r="F92" s="18"/>
-      <c r="G92" s="19"/>
+      <c r="A92" s="17"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="20"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="20"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="16"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="17"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="19"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="19"/>
+      <c r="A93" s="17"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="20"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="14"/>
-      <c r="B94" s="15"/>
-      <c r="E94" s="23"/>
-      <c r="F94" s="15"/>
-      <c r="G94" s="19"/>
+      <c r="B94" s="16"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="20"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="16"/>
-      <c r="B95" s="17"/>
-      <c r="C95" s="17"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="24"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="19"/>
+      <c r="A95" s="17"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="25"/>
+      <c r="F95" s="19"/>
+      <c r="G95" s="20"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="16"/>
-      <c r="B96" s="20"/>
-      <c r="C96" s="20"/>
-      <c r="D96" s="18"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="18"/>
-      <c r="G96" s="19"/>
+      <c r="A96" s="17"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="21"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="25"/>
+      <c r="F96" s="19"/>
+      <c r="G96" s="20"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="16"/>
-      <c r="B97" s="20"/>
-      <c r="C97" s="20"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="24"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="19"/>
+      <c r="A97" s="17"/>
+      <c r="B97" s="21"/>
+      <c r="C97" s="21"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="25"/>
+      <c r="F97" s="19"/>
+      <c r="G97" s="20"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="16"/>
-      <c r="B98" s="20"/>
-      <c r="C98" s="20"/>
-      <c r="D98" s="18"/>
-      <c r="E98" s="24"/>
-      <c r="F98" s="18"/>
-      <c r="G98" s="19"/>
+      <c r="A98" s="17"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="21"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="25"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="20"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="16"/>
-      <c r="B99" s="20"/>
-      <c r="C99" s="17"/>
-      <c r="D99" s="18"/>
-      <c r="E99" s="24"/>
-      <c r="F99" s="18"/>
-      <c r="G99" s="19"/>
+      <c r="A99" s="17"/>
+      <c r="B99" s="21"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="25"/>
+      <c r="F99" s="19"/>
+      <c r="G99" s="20"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="16"/>
-      <c r="B100" s="20"/>
-      <c r="C100" s="20"/>
-      <c r="D100" s="18"/>
-      <c r="E100" s="24"/>
-      <c r="F100" s="18"/>
-      <c r="G100" s="19"/>
+      <c r="A100" s="17"/>
+      <c r="B100" s="21"/>
+      <c r="C100" s="21"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="19"/>
+      <c r="G100" s="20"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="16"/>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="24"/>
-      <c r="F101" s="18"/>
-      <c r="G101" s="19"/>
+      <c r="A101" s="17"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="19"/>
+      <c r="G101" s="20"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="16"/>
-      <c r="B102" s="20"/>
-      <c r="C102" s="20"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="24"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="19"/>
+      <c r="A102" s="17"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="25"/>
+      <c r="F102" s="19"/>
+      <c r="G102" s="20"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="16"/>
-      <c r="B103" s="20"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="24"/>
-      <c r="F103" s="18"/>
-      <c r="G103" s="19"/>
+      <c r="A103" s="17"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="25"/>
+      <c r="F103" s="19"/>
+      <c r="G103" s="20"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="16"/>
-      <c r="B104" s="20"/>
-      <c r="C104" s="20"/>
-      <c r="D104" s="18"/>
-      <c r="E104" s="24"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="19"/>
+      <c r="A104" s="17"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="19"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="19"/>
+      <c r="G104" s="20"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="16"/>
-      <c r="B105" s="20"/>
-      <c r="C105" s="20"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="24"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="19"/>
+      <c r="A105" s="17"/>
+      <c r="B105" s="21"/>
+      <c r="C105" s="21"/>
+      <c r="D105" s="19"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="19"/>
+      <c r="G105" s="20"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="16"/>
-      <c r="B106" s="20"/>
-      <c r="C106" s="20"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="24"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="19"/>
+      <c r="A106" s="17"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="21"/>
+      <c r="D106" s="19"/>
+      <c r="E106" s="25"/>
+      <c r="F106" s="19"/>
+      <c r="G106" s="20"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="16"/>
-      <c r="B107" s="20"/>
-      <c r="C107" s="20"/>
-      <c r="D107" s="18"/>
-      <c r="E107" s="24"/>
-      <c r="F107" s="18"/>
-      <c r="G107" s="19"/>
+      <c r="A107" s="17"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="19"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="20"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="16"/>
-      <c r="B108" s="20"/>
-      <c r="C108" s="20"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="24"/>
-      <c r="F108" s="18"/>
-      <c r="G108" s="19"/>
+      <c r="A108" s="17"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="25"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="20"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="16"/>
-      <c r="B109" s="20"/>
-      <c r="C109" s="20"/>
-      <c r="D109" s="18"/>
-      <c r="E109" s="24"/>
-      <c r="F109" s="18"/>
-      <c r="G109" s="19"/>
+      <c r="A109" s="17"/>
+      <c r="B109" s="21"/>
+      <c r="C109" s="21"/>
+      <c r="D109" s="19"/>
+      <c r="E109" s="25"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="20"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="16"/>
-      <c r="B110" s="20"/>
-      <c r="C110" s="20"/>
-      <c r="D110" s="18"/>
-      <c r="E110" s="24"/>
-      <c r="F110" s="18"/>
-      <c r="G110" s="19"/>
+      <c r="A110" s="17"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="21"/>
+      <c r="D110" s="19"/>
+      <c r="E110" s="25"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="20"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="16"/>
-      <c r="B111" s="20"/>
-      <c r="C111" s="20"/>
-      <c r="D111" s="18"/>
-      <c r="E111" s="24"/>
-      <c r="F111" s="18"/>
-      <c r="G111" s="19"/>
+      <c r="A111" s="17"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="19"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="20"/>
     </row>
     <row r="112" ht="15.75" customHeight="1"/>
     <row r="113" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
added test scenarios and test cases to premier league app
</commit_message>
<xml_diff>
--- a/test_scenarios.xlsx
+++ b/test_scenarios.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James Amoani\mytechbase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James Amoani\Desktop\Documents\mytechbase_project\mytechbase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50090A31-F64D-414E-A444-BAD25155A4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133555D9-F31A-4200-8B72-208AB3C34BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
     <sheet name="Registration" sheetId="2" r:id="rId2"/>
     <sheet name="Login" sheetId="3" r:id="rId3"/>
-    <sheet name="Order assigne" sheetId="4" r:id="rId4"/>
+    <sheet name="Premier legue app" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="135">
   <si>
     <t>Project Name</t>
   </si>
@@ -262,6 +262,177 @@
   </si>
   <si>
     <t>Age below 18 years should not be registered</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User should have open to premier legue registration  page</t>
+  </si>
+  <si>
+    <t>Register using valid email adress</t>
+  </si>
+  <si>
+    <t>Enter your first name</t>
+  </si>
+  <si>
+    <t>enter your Surname</t>
+  </si>
+  <si>
+    <t>Enter a valid email adress</t>
+  </si>
+  <si>
+    <t>Enter a valid password</t>
+  </si>
+  <si>
+    <t>Enter a gender</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>Enter a invalid email adress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter a valid date of birth </t>
+  </si>
+  <si>
+    <t>Enter a valid country of residence</t>
+  </si>
+  <si>
+    <t>Register using valid date of birth</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>Enter a valid year of birth</t>
+  </si>
+  <si>
+    <t>Enter a valid month of birth</t>
+  </si>
+  <si>
+    <t>Enter a valid day of birth</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>Enter a year of birth below 18 years</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>Register using valid country code</t>
+  </si>
+  <si>
+    <t>Enter a valid country code</t>
+  </si>
+  <si>
+    <t>Check the app behavior when invalid country code is used</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <t>Enter a invalid country code</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Register using a valid phone  number</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>8.6</t>
+  </si>
+  <si>
+    <t>8.7</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>Check the app behavior when invalid phone number is used</t>
+  </si>
+  <si>
+    <t>Enter a invalid phone number</t>
+  </si>
+  <si>
+    <t>Check the app behavior  when age below is registered</t>
+  </si>
+  <si>
+    <t>Check the app behavior when invalid email is used</t>
+  </si>
+  <si>
+    <t>Redirect to login page</t>
+  </si>
+  <si>
+    <t>Email is invalid</t>
+  </si>
+  <si>
+    <t>Registration successful</t>
+  </si>
+  <si>
+    <t>Age below 18 years cannot be registered</t>
+  </si>
+  <si>
+    <t>Country code invalid</t>
+  </si>
+  <si>
+    <t>Phone number invalid</t>
   </si>
 </sst>
 </file>
@@ -410,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -492,11 +663,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -799,7 +971,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
@@ -812,46 +984,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A1" s="29"/>
-      <c r="B1" s="30"/>
+      <c r="A1" s="32"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="32"/>
+      <c r="B4" s="33"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1"/>
@@ -1869,7 +2041,7 @@
   </sheetPr>
   <dimension ref="A1:I1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -2115,11 +2287,11 @@
       <c r="A12" s="10">
         <v>2</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -2256,11 +2428,11 @@
       <c r="A19" s="10">
         <v>3</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
@@ -2366,11 +2538,11 @@
       <c r="A25" s="10">
         <v>4</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
@@ -2567,11 +2739,11 @@
       <c r="A36" s="25">
         <v>6</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
@@ -2633,9 +2805,9 @@
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1">
       <c r="A40" s="10"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
@@ -2764,9 +2936,9 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1">
       <c r="A52" s="10"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
@@ -2852,9 +3024,9 @@
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1">
       <c r="A60" s="10"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="33"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
@@ -2907,9 +3079,9 @@
     </row>
     <row r="65" spans="1:9" ht="15.75" customHeight="1">
       <c r="A65" s="10"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
@@ -2973,9 +3145,9 @@
     </row>
     <row r="71" spans="1:9" ht="15.75" customHeight="1">
       <c r="A71" s="10"/>
-      <c r="B71" s="33"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
       <c r="E71" s="12"/>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
@@ -3039,9 +3211,9 @@
     </row>
     <row r="77" spans="1:9" ht="15.75" customHeight="1">
       <c r="A77" s="10"/>
-      <c r="B77" s="33"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="33"/>
+      <c r="D77" s="33"/>
       <c r="E77" s="12"/>
       <c r="F77" s="12"/>
       <c r="G77" s="12"/>
@@ -3149,9 +3321,9 @@
     </row>
     <row r="87" spans="1:9" ht="15.75" customHeight="1">
       <c r="A87" s="10"/>
-      <c r="B87" s="33"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
+      <c r="B87" s="34"/>
+      <c r="C87" s="33"/>
+      <c r="D87" s="33"/>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
@@ -3270,9 +3442,9 @@
     </row>
     <row r="98" spans="1:9" ht="15.75" customHeight="1">
       <c r="A98" s="10"/>
-      <c r="B98" s="33"/>
-      <c r="C98" s="32"/>
-      <c r="D98" s="32"/>
+      <c r="B98" s="34"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="33"/>
       <c r="E98" s="12"/>
       <c r="F98" s="12"/>
       <c r="G98" s="12"/>
@@ -3347,9 +3519,9 @@
     </row>
     <row r="105" spans="1:9" ht="15.75" customHeight="1">
       <c r="A105" s="10"/>
-      <c r="B105" s="33"/>
-      <c r="C105" s="32"/>
-      <c r="D105" s="32"/>
+      <c r="B105" s="34"/>
+      <c r="C105" s="33"/>
+      <c r="D105" s="33"/>
       <c r="E105" s="12"/>
       <c r="F105" s="12"/>
       <c r="G105" s="12"/>
@@ -3391,9 +3563,9 @@
     </row>
     <row r="109" spans="1:9" ht="15.75" customHeight="1">
       <c r="A109" s="10"/>
-      <c r="B109" s="33"/>
-      <c r="C109" s="32"/>
-      <c r="D109" s="32"/>
+      <c r="B109" s="34"/>
+      <c r="C109" s="33"/>
+      <c r="D109" s="33"/>
       <c r="E109" s="27"/>
       <c r="F109" s="12"/>
       <c r="G109" s="16"/>
@@ -4643,9 +4815,9 @@
       <c r="A7" s="10">
         <v>2</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -4709,9 +4881,9 @@
       <c r="A11" s="10">
         <v>3</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -4775,9 +4947,9 @@
       <c r="A15" s="10">
         <v>4</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -4887,9 +5059,9 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
       <c r="A22" s="10"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
@@ -4917,9 +5089,9 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
       <c r="A25" s="10"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
@@ -5036,9 +5208,9 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
       <c r="A37" s="10"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
@@ -5116,9 +5288,9 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1">
       <c r="A45" s="10"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -5166,9 +5338,9 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1">
       <c r="A50" s="10"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
@@ -5226,9 +5398,9 @@
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1">
       <c r="A56" s="10"/>
-      <c r="B56" s="33"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
@@ -5286,9 +5458,9 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1">
       <c r="A62" s="10"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="33"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
@@ -5386,9 +5558,9 @@
     </row>
     <row r="72" spans="1:8" ht="15.75" customHeight="1">
       <c r="A72" s="10"/>
-      <c r="B72" s="33"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="33"/>
       <c r="E72" s="12"/>
       <c r="F72" s="12"/>
       <c r="G72" s="12"/>
@@ -5496,9 +5668,9 @@
     </row>
     <row r="83" spans="1:8" ht="15.75" customHeight="1">
       <c r="A83" s="10"/>
-      <c r="B83" s="33"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="32"/>
+      <c r="B83" s="34"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="33"/>
       <c r="E83" s="12"/>
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
@@ -5566,9 +5738,9 @@
     </row>
     <row r="90" spans="1:8" ht="15.75" customHeight="1">
       <c r="A90" s="10"/>
-      <c r="B90" s="33"/>
-      <c r="C90" s="32"/>
-      <c r="D90" s="32"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
@@ -5606,9 +5778,9 @@
     </row>
     <row r="94" spans="1:8" ht="15.75" customHeight="1">
       <c r="A94" s="10"/>
-      <c r="B94" s="33"/>
-      <c r="C94" s="32"/>
-      <c r="D94" s="32"/>
+      <c r="B94" s="34"/>
+      <c r="C94" s="33"/>
+      <c r="D94" s="33"/>
       <c r="E94" s="27"/>
       <c r="F94" s="12"/>
       <c r="G94" s="16"/>
@@ -6720,9 +6892,11 @@
     <tabColor rgb="FFF1C232"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H1000"/>
+  <dimension ref="A1:H1028"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -6765,7 +6939,9 @@
       <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -6777,7 +6953,9 @@
       <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
@@ -6789,7 +6967,9 @@
       <c r="A4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="C4" s="14"/>
       <c r="D4" s="15" t="s">
         <v>66</v>
@@ -6807,7 +6987,9 @@
       <c r="A5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="17"/>
+      <c r="B5" s="17" t="s">
+        <v>81</v>
+      </c>
       <c r="C5" s="17"/>
       <c r="D5" s="15" t="s">
         <v>21</v>
@@ -6821,78 +7003,88 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="15" t="s">
+      <c r="B6" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="16"/>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="20" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A7" s="10">
-        <v>2</v>
-      </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15" t="s">
+      <c r="H6" s="20"/>
+    </row>
+    <row r="7" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="16"/>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="20" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="16"/>
-      <c r="H8" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15" t="s">
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="16"/>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="20" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="16"/>
-      <c r="H9" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="14"/>
+        <v>32</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="17"/>
       <c r="D10" s="15" t="s">
         <v>21</v>
       </c>
@@ -6907,11 +7099,13 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="A11" s="10">
-        <v>3</v>
-      </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
+        <v>2</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -6919,9 +7113,11 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="22"/>
+        <v>37</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>80</v>
+      </c>
       <c r="C12" s="14"/>
       <c r="D12" s="15" t="s">
         <v>21</v>
@@ -6937,9 +7133,11 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="22"/>
+        <v>39</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="C13" s="14"/>
       <c r="D13" s="15" t="s">
         <v>21</v>
@@ -6953,96 +7151,106 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A14" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15" t="s">
+    <row r="14" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="16"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="20" t="s">
         <v>21</v>
       </c>
       <c r="G14" s="16"/>
-      <c r="H14" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A15" s="10">
-        <v>4</v>
-      </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A16" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15" t="s">
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="D15" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="20" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="16"/>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="20" t="s">
         <v>21</v>
       </c>
       <c r="G16" s="16"/>
-      <c r="H16" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A17" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15" t="s">
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A17" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="20" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="16"/>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="20" t="s">
         <v>21</v>
       </c>
       <c r="G17" s="16"/>
-      <c r="H17" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A18" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15" t="s">
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A18" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="20" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="16"/>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="20" t="s">
         <v>21</v>
       </c>
       <c r="G18" s="16"/>
-      <c r="H18" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
+        <v>86</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="14"/>
       <c r="D19" s="15" t="s">
         <v>21</v>
       </c>
@@ -7057,11 +7265,13 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1">
       <c r="A20" s="10">
-        <v>5</v>
-      </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+        <v>3</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
@@ -7069,9 +7279,11 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1">
       <c r="A21" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="14"/>
+        <v>46</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>80</v>
+      </c>
       <c r="C21" s="14"/>
       <c r="D21" s="15" t="s">
         <v>21</v>
@@ -7086,448 +7298,786 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="15"/>
+      <c r="A22" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="24"/>
+      <c r="D23" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E23" s="16"/>
-      <c r="F23" s="15"/>
+      <c r="F23" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
+      <c r="H23" s="20"/>
+    </row>
+    <row r="24" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A24" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E24" s="16"/>
-      <c r="F24" s="15"/>
+      <c r="F24" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A25" s="10"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A26" s="13"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15"/>
+      <c r="H24" s="20"/>
+    </row>
+    <row r="25" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A25" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A26" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="24"/>
+      <c r="D26" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E26" s="16"/>
-      <c r="F26" s="15"/>
+      <c r="F26" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14"/>
+      <c r="A27" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>94</v>
+      </c>
       <c r="C27" s="14"/>
-      <c r="D27" s="15"/>
+      <c r="D27" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="E27" s="16"/>
-      <c r="F27" s="15"/>
+      <c r="F27" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
+      <c r="H27" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A28" s="10"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
+      <c r="A28" s="10">
+        <v>4</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
+      <c r="A29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="E29" s="16"/>
-      <c r="F29" s="15"/>
+      <c r="F29" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="H29" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A30" s="13"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="15"/>
+      <c r="A30" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="E30" s="16"/>
-      <c r="F30" s="15"/>
+      <c r="F30" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
+      <c r="H30" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A31" s="13"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="15"/>
+      <c r="A31" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="E31" s="16"/>
-      <c r="F31" s="15"/>
+      <c r="F31" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="H31" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
-      <c r="D32" s="15"/>
+      <c r="D32" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="E32" s="16"/>
-      <c r="F32" s="15"/>
+      <c r="F32" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
+      <c r="H32" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A33" s="13"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="A33" s="10">
+        <v>5</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A34" s="13"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="15"/>
+      <c r="A34" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="E34" s="16"/>
-      <c r="F34" s="15"/>
+      <c r="F34" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A35" s="13"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="15"/>
+      <c r="H34" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A35" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="24"/>
+      <c r="D35" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E35" s="16"/>
-      <c r="F35" s="15"/>
+      <c r="F35" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A36" s="13"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="H35" s="20"/>
+    </row>
+    <row r="36" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A36" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="24"/>
+      <c r="D36" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="16"/>
+      <c r="F36" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A37" s="10"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A38" s="13"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="15"/>
+      <c r="H36" s="20"/>
+    </row>
+    <row r="37" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A37" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="24"/>
+      <c r="D37" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="16"/>
+      <c r="F37" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="16"/>
+      <c r="H37" s="20"/>
+    </row>
+    <row r="38" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A38" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E38" s="16"/>
-      <c r="F38" s="15"/>
+      <c r="F38" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A39" s="13"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="15"/>
+      <c r="H38" s="20"/>
+    </row>
+    <row r="39" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A39" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="24"/>
+      <c r="D39" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E39" s="16"/>
-      <c r="F39" s="15"/>
+      <c r="F39" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A40" s="13"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="15"/>
+      <c r="H39" s="20"/>
+    </row>
+    <row r="40" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A40" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E40" s="16"/>
-      <c r="F40" s="15"/>
+      <c r="F40" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
+      <c r="H40" s="20"/>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A41" s="13"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="A41" s="10">
+        <v>6</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A42" s="13"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="15"/>
+      <c r="A42" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="E42" s="16"/>
-      <c r="F42" s="15"/>
+      <c r="F42" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
     </row>
-    <row r="43" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A43" s="13"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="15"/>
+    <row r="43" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A43" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="24"/>
+      <c r="D43" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E43" s="16"/>
-      <c r="F43" s="15"/>
+      <c r="F43" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A44" s="13"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="15"/>
+    <row r="44" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A44" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="24"/>
+      <c r="D44" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E44" s="16"/>
-      <c r="F44" s="15"/>
+      <c r="F44" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
     </row>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A45" s="10"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A46" s="13"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="15"/>
+    <row r="45" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A45" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="24"/>
+      <c r="D45" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="16"/>
+      <c r="F45" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+    </row>
+    <row r="46" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A46" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E46" s="16"/>
-      <c r="F46" s="15"/>
+      <c r="F46" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
     </row>
-    <row r="47" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A47" s="13"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="15"/>
+    <row r="47" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A47" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="24"/>
+      <c r="D47" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E47" s="16"/>
-      <c r="F47" s="15"/>
+      <c r="F47" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A48" s="13"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="15"/>
+      <c r="A48" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E48" s="16"/>
-      <c r="F48" s="15"/>
+      <c r="F48" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G48" s="16"/>
       <c r="H48" s="16"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A49" s="13"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
+      <c r="A49" s="10">
+        <v>7</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A50" s="10"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A51" s="13"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="15"/>
+      <c r="A50" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="16"/>
+      <c r="F50" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A51" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="24"/>
+      <c r="D51" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E51" s="16"/>
-      <c r="F51" s="15"/>
+      <c r="F51" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
     </row>
-    <row r="52" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A52" s="13"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="15"/>
+    <row r="52" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A52" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E52" s="16"/>
-      <c r="F52" s="15"/>
+      <c r="F52" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
     </row>
-    <row r="53" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A53" s="13"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="15"/>
+    <row r="53" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A53" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" s="24"/>
+      <c r="D53" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E53" s="16"/>
-      <c r="F53" s="15"/>
+      <c r="F53" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G53" s="16"/>
       <c r="H53" s="16"/>
     </row>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A54" s="13"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="15"/>
+    <row r="54" spans="1:8" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A54" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="24"/>
+      <c r="D54" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E54" s="16"/>
-      <c r="F54" s="15"/>
+      <c r="F54" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A55" s="13"/>
-      <c r="B55" s="17"/>
+      <c r="A55" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>88</v>
+      </c>
       <c r="C55" s="14"/>
-      <c r="D55" s="15"/>
+      <c r="D55" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E55" s="16"/>
-      <c r="F55" s="15"/>
+      <c r="F55" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G55" s="16"/>
       <c r="H55" s="16"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A56" s="10"/>
-      <c r="B56" s="33"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
+      <c r="A56" s="10">
+        <v>8</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A57" s="13"/>
-      <c r="B57" s="14"/>
+      <c r="A57" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>80</v>
+      </c>
       <c r="C57" s="14"/>
-      <c r="D57" s="15"/>
+      <c r="D57" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="E57" s="16"/>
-      <c r="F57" s="15"/>
+      <c r="F57" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="G57" s="16"/>
       <c r="H57" s="16"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A58" s="13"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="15"/>
+      <c r="A58" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="17"/>
+      <c r="D58" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E58" s="16"/>
-      <c r="F58" s="15"/>
+      <c r="F58" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G58" s="16"/>
       <c r="H58" s="16"/>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A59" s="13"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="15"/>
+      <c r="A59" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E59" s="16"/>
-      <c r="F59" s="15"/>
+      <c r="F59" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G59" s="16"/>
       <c r="H59" s="16"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A60" s="13"/>
-      <c r="B60" s="17"/>
+      <c r="A60" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>83</v>
+      </c>
       <c r="C60" s="17"/>
-      <c r="D60" s="15"/>
+      <c r="D60" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E60" s="16"/>
-      <c r="F60" s="15"/>
+      <c r="F60" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G60" s="16"/>
       <c r="H60" s="16"/>
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A61" s="13"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="15"/>
+      <c r="A61" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" s="17"/>
+      <c r="D61" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E61" s="16"/>
-      <c r="F61" s="15"/>
+      <c r="F61" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G61" s="16"/>
       <c r="H61" s="16"/>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A62" s="10"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
+      <c r="A62" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" s="17"/>
+      <c r="D62" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="16"/>
+      <c r="F62" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A63" s="13"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="15"/>
+      <c r="A63" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E63" s="16"/>
-      <c r="F63" s="15"/>
+      <c r="F63" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G63" s="16"/>
       <c r="H63" s="16"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A64" s="13"/>
+      <c r="A64" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="B64" s="17"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="15"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="G64" s="16"/>
       <c r="H64" s="16"/>
     </row>
     <row r="65" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A65" s="13"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
+      <c r="A65" s="10"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
     </row>
     <row r="66" spans="1:8" ht="15.75" customHeight="1">
       <c r="A66" s="13"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
       <c r="D66" s="15"/>
       <c r="E66" s="16"/>
       <c r="F66" s="15"/>
@@ -7537,7 +8087,7 @@
     <row r="67" spans="1:8" ht="15.75" customHeight="1">
       <c r="A67" s="13"/>
       <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
+      <c r="C67" s="14"/>
       <c r="D67" s="15"/>
       <c r="E67" s="16"/>
       <c r="F67" s="15"/>
@@ -7585,28 +8135,28 @@
       <c r="H71" s="16"/>
     </row>
     <row r="72" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A72" s="10"/>
-      <c r="B72" s="33"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
     </row>
     <row r="73" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A73" s="13"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="16"/>
+      <c r="A73" s="10"/>
+      <c r="B73" s="34"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="33"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
     </row>
     <row r="74" spans="1:8" ht="15.75" customHeight="1">
       <c r="A74" s="13"/>
-      <c r="B74" s="17"/>
+      <c r="B74" s="14"/>
       <c r="C74" s="14"/>
       <c r="D74" s="15"/>
       <c r="E74" s="16"/>
@@ -7617,7 +8167,7 @@
     <row r="75" spans="1:8" ht="15.75" customHeight="1">
       <c r="A75" s="13"/>
       <c r="B75" s="17"/>
-      <c r="C75" s="14"/>
+      <c r="C75" s="17"/>
       <c r="D75" s="15"/>
       <c r="E75" s="16"/>
       <c r="F75" s="15"/>
@@ -7637,7 +8187,7 @@
     <row r="77" spans="1:8" ht="15.75" customHeight="1">
       <c r="A77" s="13"/>
       <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
+      <c r="C77" s="14"/>
       <c r="D77" s="15"/>
       <c r="E77" s="16"/>
       <c r="F77" s="15"/>
@@ -7645,19 +8195,19 @@
       <c r="H77" s="16"/>
     </row>
     <row r="78" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A78" s="13"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="16"/>
-      <c r="H78" s="16"/>
+      <c r="A78" s="10"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
     </row>
     <row r="79" spans="1:8" ht="15.75" customHeight="1">
       <c r="A79" s="13"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="17"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
       <c r="D79" s="15"/>
       <c r="E79" s="16"/>
       <c r="F79" s="15"/>
@@ -7667,7 +8217,7 @@
     <row r="80" spans="1:8" ht="15.75" customHeight="1">
       <c r="A80" s="13"/>
       <c r="B80" s="17"/>
-      <c r="C80" s="17"/>
+      <c r="C80" s="14"/>
       <c r="D80" s="15"/>
       <c r="E80" s="16"/>
       <c r="F80" s="15"/>
@@ -7677,7 +8227,7 @@
     <row r="81" spans="1:8" ht="15.75" customHeight="1">
       <c r="A81" s="13"/>
       <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
+      <c r="C81" s="14"/>
       <c r="D81" s="15"/>
       <c r="E81" s="16"/>
       <c r="F81" s="15"/>
@@ -7695,29 +8245,29 @@
       <c r="H82" s="16"/>
     </row>
     <row r="83" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A83" s="10"/>
-      <c r="B83" s="33"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="32"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
+      <c r="A83" s="13"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="16"/>
     </row>
     <row r="84" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A84" s="13"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="15"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="15"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="34"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
     </row>
     <row r="85" spans="1:8" ht="15.75" customHeight="1">
       <c r="A85" s="13"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="17"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
       <c r="D85" s="15"/>
       <c r="E85" s="16"/>
       <c r="F85" s="15"/>
@@ -7727,7 +8277,7 @@
     <row r="86" spans="1:8" ht="15.75" customHeight="1">
       <c r="A86" s="13"/>
       <c r="B86" s="17"/>
-      <c r="C86" s="17"/>
+      <c r="C86" s="14"/>
       <c r="D86" s="15"/>
       <c r="E86" s="16"/>
       <c r="F86" s="15"/>
@@ -7737,7 +8287,7 @@
     <row r="87" spans="1:8" ht="15.75" customHeight="1">
       <c r="A87" s="13"/>
       <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
+      <c r="C87" s="14"/>
       <c r="D87" s="15"/>
       <c r="E87" s="16"/>
       <c r="F87" s="15"/>
@@ -7757,7 +8307,7 @@
     <row r="89" spans="1:8" ht="15.75" customHeight="1">
       <c r="A89" s="13"/>
       <c r="B89" s="17"/>
-      <c r="C89" s="17"/>
+      <c r="C89" s="14"/>
       <c r="D89" s="15"/>
       <c r="E89" s="16"/>
       <c r="F89" s="15"/>
@@ -7766,9 +8316,9 @@
     </row>
     <row r="90" spans="1:8" ht="15.75" customHeight="1">
       <c r="A90" s="10"/>
-      <c r="B90" s="33"/>
-      <c r="C90" s="32"/>
-      <c r="D90" s="32"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
@@ -7776,7 +8326,7 @@
     </row>
     <row r="91" spans="1:8" ht="15.75" customHeight="1">
       <c r="A91" s="13"/>
-      <c r="B91" s="22"/>
+      <c r="B91" s="14"/>
       <c r="C91" s="14"/>
       <c r="D91" s="15"/>
       <c r="E91" s="16"/>
@@ -7786,7 +8336,7 @@
     </row>
     <row r="92" spans="1:8" ht="15.75" customHeight="1">
       <c r="A92" s="13"/>
-      <c r="B92" s="22"/>
+      <c r="B92" s="17"/>
       <c r="C92" s="14"/>
       <c r="D92" s="15"/>
       <c r="E92" s="16"/>
@@ -7796,7 +8346,7 @@
     </row>
     <row r="93" spans="1:8" ht="15.75" customHeight="1">
       <c r="A93" s="13"/>
-      <c r="B93" s="22"/>
+      <c r="B93" s="17"/>
       <c r="C93" s="14"/>
       <c r="D93" s="15"/>
       <c r="E93" s="16"/>
@@ -7805,21 +8355,21 @@
       <c r="H93" s="16"/>
     </row>
     <row r="94" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A94" s="10"/>
-      <c r="B94" s="33"/>
-      <c r="C94" s="32"/>
-      <c r="D94" s="32"/>
-      <c r="E94" s="27"/>
-      <c r="F94" s="12"/>
+      <c r="A94" s="13"/>
+      <c r="B94" s="17"/>
+      <c r="C94" s="17"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="16"/>
+      <c r="F94" s="15"/>
       <c r="G94" s="16"/>
       <c r="H94" s="16"/>
     </row>
     <row r="95" spans="1:8" ht="15.75" customHeight="1">
       <c r="A95" s="13"/>
-      <c r="B95" s="14"/>
-      <c r="C95" s="14"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="17"/>
       <c r="D95" s="15"/>
-      <c r="E95" s="28"/>
+      <c r="E95" s="16"/>
       <c r="F95" s="15"/>
       <c r="G95" s="16"/>
       <c r="H95" s="16"/>
@@ -7829,7 +8379,7 @@
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>
       <c r="D96" s="15"/>
-      <c r="E96" s="28"/>
+      <c r="E96" s="16"/>
       <c r="F96" s="15"/>
       <c r="G96" s="16"/>
       <c r="H96" s="16"/>
@@ -7839,7 +8389,7 @@
       <c r="B97" s="17"/>
       <c r="C97" s="17"/>
       <c r="D97" s="15"/>
-      <c r="E97" s="28"/>
+      <c r="E97" s="16"/>
       <c r="F97" s="15"/>
       <c r="G97" s="16"/>
       <c r="H97" s="16"/>
@@ -7849,7 +8399,7 @@
       <c r="B98" s="17"/>
       <c r="C98" s="17"/>
       <c r="D98" s="15"/>
-      <c r="E98" s="28"/>
+      <c r="E98" s="16"/>
       <c r="F98" s="15"/>
       <c r="G98" s="16"/>
       <c r="H98" s="16"/>
@@ -7857,29 +8407,29 @@
     <row r="99" spans="1:8" ht="15.75" customHeight="1">
       <c r="A99" s="13"/>
       <c r="B99" s="17"/>
-      <c r="C99" s="14"/>
+      <c r="C99" s="17"/>
       <c r="D99" s="15"/>
-      <c r="E99" s="28"/>
+      <c r="E99" s="16"/>
       <c r="F99" s="15"/>
       <c r="G99" s="16"/>
       <c r="H99" s="16"/>
     </row>
     <row r="100" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A100" s="13"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="17"/>
-      <c r="D100" s="15"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="15"/>
-      <c r="G100" s="16"/>
-      <c r="H100" s="16"/>
+      <c r="A100" s="10"/>
+      <c r="B100" s="34"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="12"/>
     </row>
     <row r="101" spans="1:8" ht="15.75" customHeight="1">
       <c r="A101" s="13"/>
-      <c r="B101" s="17"/>
-      <c r="C101" s="17"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
       <c r="D101" s="15"/>
-      <c r="E101" s="28"/>
+      <c r="E101" s="16"/>
       <c r="F101" s="15"/>
       <c r="G101" s="16"/>
       <c r="H101" s="16"/>
@@ -7887,9 +8437,9 @@
     <row r="102" spans="1:8" ht="15.75" customHeight="1">
       <c r="A102" s="13"/>
       <c r="B102" s="17"/>
-      <c r="C102" s="17"/>
+      <c r="C102" s="14"/>
       <c r="D102" s="15"/>
-      <c r="E102" s="28"/>
+      <c r="E102" s="16"/>
       <c r="F102" s="15"/>
       <c r="G102" s="16"/>
       <c r="H102" s="16"/>
@@ -7899,7 +8449,7 @@
       <c r="B103" s="17"/>
       <c r="C103" s="14"/>
       <c r="D103" s="15"/>
-      <c r="E103" s="28"/>
+      <c r="E103" s="16"/>
       <c r="F103" s="15"/>
       <c r="G103" s="16"/>
       <c r="H103" s="16"/>
@@ -7909,7 +8459,7 @@
       <c r="B104" s="17"/>
       <c r="C104" s="17"/>
       <c r="D104" s="15"/>
-      <c r="E104" s="28"/>
+      <c r="E104" s="16"/>
       <c r="F104" s="15"/>
       <c r="G104" s="16"/>
       <c r="H104" s="16"/>
@@ -7919,7 +8469,7 @@
       <c r="B105" s="17"/>
       <c r="C105" s="17"/>
       <c r="D105" s="15"/>
-      <c r="E105" s="28"/>
+      <c r="E105" s="16"/>
       <c r="F105" s="15"/>
       <c r="G105" s="16"/>
       <c r="H105" s="16"/>
@@ -7929,7 +8479,7 @@
       <c r="B106" s="17"/>
       <c r="C106" s="17"/>
       <c r="D106" s="15"/>
-      <c r="E106" s="28"/>
+      <c r="E106" s="16"/>
       <c r="F106" s="15"/>
       <c r="G106" s="16"/>
       <c r="H106" s="16"/>
@@ -7939,7 +8489,7 @@
       <c r="B107" s="17"/>
       <c r="C107" s="17"/>
       <c r="D107" s="15"/>
-      <c r="E107" s="28"/>
+      <c r="E107" s="16"/>
       <c r="F107" s="15"/>
       <c r="G107" s="16"/>
       <c r="H107" s="16"/>
@@ -7949,7 +8499,7 @@
       <c r="B108" s="17"/>
       <c r="C108" s="17"/>
       <c r="D108" s="15"/>
-      <c r="E108" s="28"/>
+      <c r="E108" s="16"/>
       <c r="F108" s="15"/>
       <c r="G108" s="16"/>
       <c r="H108" s="16"/>
@@ -7959,7 +8509,7 @@
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
       <c r="D109" s="15"/>
-      <c r="E109" s="28"/>
+      <c r="E109" s="16"/>
       <c r="F109" s="15"/>
       <c r="G109" s="16"/>
       <c r="H109" s="16"/>
@@ -7969,54 +8519,306 @@
       <c r="B110" s="17"/>
       <c r="C110" s="17"/>
       <c r="D110" s="15"/>
-      <c r="E110" s="28"/>
+      <c r="E110" s="16"/>
       <c r="F110" s="15"/>
       <c r="G110" s="16"/>
       <c r="H110" s="16"/>
     </row>
     <row r="111" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A111" s="13"/>
-      <c r="B111" s="17"/>
-      <c r="C111" s="17"/>
-      <c r="D111" s="15"/>
-      <c r="E111" s="28"/>
-      <c r="F111" s="15"/>
-      <c r="G111" s="16"/>
-      <c r="H111" s="16"/>
-    </row>
-    <row r="112" spans="1:8" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
+      <c r="A111" s="10"/>
+      <c r="B111" s="34"/>
+      <c r="C111" s="33"/>
+      <c r="D111" s="33"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+      <c r="G111" s="12"/>
+      <c r="H111" s="12"/>
+    </row>
+    <row r="112" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A112" s="13"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="14"/>
+      <c r="D112" s="15"/>
+      <c r="E112" s="16"/>
+      <c r="F112" s="15"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
+    </row>
+    <row r="113" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A113" s="13"/>
+      <c r="B113" s="17"/>
+      <c r="C113" s="17"/>
+      <c r="D113" s="15"/>
+      <c r="E113" s="16"/>
+      <c r="F113" s="15"/>
+      <c r="G113" s="16"/>
+      <c r="H113" s="16"/>
+    </row>
+    <row r="114" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A114" s="13"/>
+      <c r="B114" s="17"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="15"/>
+      <c r="E114" s="16"/>
+      <c r="F114" s="15"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="16"/>
+    </row>
+    <row r="115" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A115" s="13"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="17"/>
+      <c r="D115" s="15"/>
+      <c r="E115" s="16"/>
+      <c r="F115" s="15"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="16"/>
+    </row>
+    <row r="116" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A116" s="13"/>
+      <c r="B116" s="17"/>
+      <c r="C116" s="17"/>
+      <c r="D116" s="15"/>
+      <c r="E116" s="16"/>
+      <c r="F116" s="15"/>
+      <c r="G116" s="16"/>
+      <c r="H116" s="16"/>
+    </row>
+    <row r="117" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A117" s="13"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="17"/>
+      <c r="D117" s="15"/>
+      <c r="E117" s="16"/>
+      <c r="F117" s="15"/>
+      <c r="G117" s="16"/>
+      <c r="H117" s="16"/>
+    </row>
+    <row r="118" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A118" s="10"/>
+      <c r="B118" s="34"/>
+      <c r="C118" s="33"/>
+      <c r="D118" s="33"/>
+      <c r="E118" s="12"/>
+      <c r="F118" s="12"/>
+      <c r="G118" s="12"/>
+      <c r="H118" s="12"/>
+    </row>
+    <row r="119" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A119" s="13"/>
+      <c r="B119" s="22"/>
+      <c r="C119" s="14"/>
+      <c r="D119" s="15"/>
+      <c r="E119" s="16"/>
+      <c r="F119" s="15"/>
+      <c r="G119" s="16"/>
+      <c r="H119" s="16"/>
+    </row>
+    <row r="120" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A120" s="13"/>
+      <c r="B120" s="22"/>
+      <c r="C120" s="14"/>
+      <c r="D120" s="15"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="15"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="16"/>
+    </row>
+    <row r="121" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A121" s="13"/>
+      <c r="B121" s="22"/>
+      <c r="C121" s="14"/>
+      <c r="D121" s="15"/>
+      <c r="E121" s="16"/>
+      <c r="F121" s="15"/>
+      <c r="G121" s="16"/>
+      <c r="H121" s="16"/>
+    </row>
+    <row r="122" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A122" s="10"/>
+      <c r="B122" s="34"/>
+      <c r="C122" s="33"/>
+      <c r="D122" s="33"/>
+      <c r="E122" s="27"/>
+      <c r="F122" s="12"/>
+      <c r="G122" s="16"/>
+      <c r="H122" s="16"/>
+    </row>
+    <row r="123" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A123" s="13"/>
+      <c r="B123" s="14"/>
+      <c r="C123" s="14"/>
+      <c r="D123" s="15"/>
+      <c r="E123" s="28"/>
+      <c r="F123" s="15"/>
+      <c r="G123" s="16"/>
+      <c r="H123" s="16"/>
+    </row>
+    <row r="124" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A124" s="13"/>
+      <c r="B124" s="17"/>
+      <c r="C124" s="17"/>
+      <c r="D124" s="15"/>
+      <c r="E124" s="28"/>
+      <c r="F124" s="15"/>
+      <c r="G124" s="16"/>
+      <c r="H124" s="16"/>
+    </row>
+    <row r="125" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A125" s="13"/>
+      <c r="B125" s="17"/>
+      <c r="C125" s="17"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="28"/>
+      <c r="F125" s="15"/>
+      <c r="G125" s="16"/>
+      <c r="H125" s="16"/>
+    </row>
+    <row r="126" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A126" s="13"/>
+      <c r="B126" s="17"/>
+      <c r="C126" s="17"/>
+      <c r="D126" s="15"/>
+      <c r="E126" s="28"/>
+      <c r="F126" s="15"/>
+      <c r="G126" s="16"/>
+      <c r="H126" s="16"/>
+    </row>
+    <row r="127" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A127" s="13"/>
+      <c r="B127" s="17"/>
+      <c r="C127" s="14"/>
+      <c r="D127" s="15"/>
+      <c r="E127" s="28"/>
+      <c r="F127" s="15"/>
+      <c r="G127" s="16"/>
+      <c r="H127" s="16"/>
+    </row>
+    <row r="128" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A128" s="13"/>
+      <c r="B128" s="17"/>
+      <c r="C128" s="17"/>
+      <c r="D128" s="15"/>
+      <c r="E128" s="28"/>
+      <c r="F128" s="15"/>
+      <c r="G128" s="16"/>
+      <c r="H128" s="16"/>
+    </row>
+    <row r="129" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A129" s="13"/>
+      <c r="B129" s="17"/>
+      <c r="C129" s="17"/>
+      <c r="D129" s="15"/>
+      <c r="E129" s="28"/>
+      <c r="F129" s="15"/>
+      <c r="G129" s="16"/>
+      <c r="H129" s="16"/>
+    </row>
+    <row r="130" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A130" s="13"/>
+      <c r="B130" s="17"/>
+      <c r="C130" s="17"/>
+      <c r="D130" s="15"/>
+      <c r="E130" s="28"/>
+      <c r="F130" s="15"/>
+      <c r="G130" s="16"/>
+      <c r="H130" s="16"/>
+    </row>
+    <row r="131" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A131" s="13"/>
+      <c r="B131" s="17"/>
+      <c r="C131" s="14"/>
+      <c r="D131" s="15"/>
+      <c r="E131" s="28"/>
+      <c r="F131" s="15"/>
+      <c r="G131" s="16"/>
+      <c r="H131" s="16"/>
+    </row>
+    <row r="132" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A132" s="13"/>
+      <c r="B132" s="17"/>
+      <c r="C132" s="17"/>
+      <c r="D132" s="15"/>
+      <c r="E132" s="28"/>
+      <c r="F132" s="15"/>
+      <c r="G132" s="16"/>
+      <c r="H132" s="16"/>
+    </row>
+    <row r="133" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A133" s="13"/>
+      <c r="B133" s="17"/>
+      <c r="C133" s="17"/>
+      <c r="D133" s="15"/>
+      <c r="E133" s="28"/>
+      <c r="F133" s="15"/>
+      <c r="G133" s="16"/>
+      <c r="H133" s="16"/>
+    </row>
+    <row r="134" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A134" s="13"/>
+      <c r="B134" s="17"/>
+      <c r="C134" s="17"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="28"/>
+      <c r="F134" s="15"/>
+      <c r="G134" s="16"/>
+      <c r="H134" s="16"/>
+    </row>
+    <row r="135" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A135" s="13"/>
+      <c r="B135" s="17"/>
+      <c r="C135" s="17"/>
+      <c r="D135" s="15"/>
+      <c r="E135" s="28"/>
+      <c r="F135" s="15"/>
+      <c r="G135" s="16"/>
+      <c r="H135" s="16"/>
+    </row>
+    <row r="136" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A136" s="13"/>
+      <c r="B136" s="17"/>
+      <c r="C136" s="17"/>
+      <c r="D136" s="15"/>
+      <c r="E136" s="28"/>
+      <c r="F136" s="15"/>
+      <c r="G136" s="16"/>
+      <c r="H136" s="16"/>
+    </row>
+    <row r="137" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A137" s="13"/>
+      <c r="B137" s="17"/>
+      <c r="C137" s="17"/>
+      <c r="D137" s="15"/>
+      <c r="E137" s="28"/>
+      <c r="F137" s="15"/>
+      <c r="G137" s="16"/>
+      <c r="H137" s="16"/>
+    </row>
+    <row r="138" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A138" s="13"/>
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="15"/>
+      <c r="E138" s="28"/>
+      <c r="F138" s="15"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="16"/>
+    </row>
+    <row r="139" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A139" s="13"/>
+      <c r="B139" s="17"/>
+      <c r="C139" s="17"/>
+      <c r="D139" s="15"/>
+      <c r="E139" s="28"/>
+      <c r="F139" s="15"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="16"/>
+    </row>
+    <row r="140" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="141" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="142" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="143" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="144" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="145" ht="15.75" customHeight="1"/>
     <row r="146" ht="15.75" customHeight="1"/>
     <row r="147" ht="15.75" customHeight="1"/>
@@ -8873,40 +9675,68 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
+    <row r="1016" ht="15.75" customHeight="1"/>
+    <row r="1017" ht="15.75" customHeight="1"/>
+    <row r="1018" ht="15.75" customHeight="1"/>
+    <row r="1019" ht="15.75" customHeight="1"/>
+    <row r="1020" ht="15.75" customHeight="1"/>
+    <row r="1021" ht="15.75" customHeight="1"/>
+    <row r="1022" ht="15.75" customHeight="1"/>
+    <row r="1023" ht="15.75" customHeight="1"/>
+    <row r="1024" ht="15.75" customHeight="1"/>
+    <row r="1025" ht="15.75" customHeight="1"/>
+    <row r="1026" ht="15.75" customHeight="1"/>
+    <row r="1027" ht="15.75" customHeight="1"/>
+    <row r="1028" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B122:D122"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B84:D84"/>
     <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="B111:D111"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:D6 D8:D10 D12:D14 D16:D19 D21 D23:D24 D26:D27 D29:D36 D38:D44 D46:D49 D51:D55 D57:D61 D63:D71 D73:D82 D84:D89 D91:D93 D95:D111 F4:F6 F8:F10 F12:F14 F16:F19 F21 F23:F24 F26:F27 F29:F36 F38:F44 F46:F49 F51:F55 F57:F61 F63:F71 F73:F82 F84:F89 F91:F111 H4:H6 H8:H10 H12:H14 H16:H19 H21">
+  <conditionalFormatting sqref="D29:D32 D66:D72 D74:D77 D79:D83 D85:D89 D91:D99 D101:D110 D112:D117 D119:D121 D123:D139 F29:F32 F66:F72 F74:F77 F79:F83 F85:F89 F91:F99 F101:F110 F112:F117 F119:F139 H4:H10 H12:H19 H21:H27 H29:H32 H34:H40 D4:D10 F4:F10 D12:D19 F12:F19 D21:D27 F21:F27 D34:D40 F34:F40 D42:D48 F42:F48 D50:D55 F50:F55 D57:D64 F57:F64">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D6 D8:D10 D12:D14 D16:D19 D21 D23:D24 D26:D27 D29:D36 D38:D44 D46:D49 D51:D55 D57:D61 D63:D71 D73:D82 D84:D89 D91:D93 D95:D111 F4:F6 F8:F10 F12:F14 F16:F19 F21 F23:F24 F26:F27 F29:F36 F38:F44 F46:F49 F51:F55 F57:F61 F63:F71 F73:F82 F84:F89 F91:F111 H4:H6 H8:H10 H12:H14 H16:H19 H21">
+  <conditionalFormatting sqref="D29:D32 D66:D72 D74:D77 D79:D83 D85:D89 D91:D99 D101:D110 D112:D117 D119:D121 D123:D139 F29:F32 F66:F72 F74:F77 F79:F83 F85:F89 F91:F99 F101:F110 F112:F117 F119:F139 H4:H10 H12:H19 H21:H27 H29:H32 H34:H40 D4:D10 F4:F10 D12:D19 F12:F19 D21:D27 F21:F27 D34:D40 F34:F40 D42:D48 F42:F48 D50:D55 F50:F55 D57:D64 F57:F64">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D6 D8:D10 D12:D14 D16:D19 D21 D23:D24 D26:D27 D29:D36 D38:D44 D46:D49 D51:D55 D57:D61 D63:D71 D73:D82 D84:D89 D91:D93 D95:D111 F4:F6 F8:F10 F12:F14 F16:F19 F21 F23:F24 F26:F27 F29:F36 F38:F44 F46:F49 F51:F55 F57:F61 F63:F71 F73:F82 F84:F89 F91:F111 H4:H6 H8:H10 H12:H14 H16:H19 H21">
+  <conditionalFormatting sqref="D29:D32 D66:D72 D74:D77 D79:D83 D85:D89 D91:D99 D101:D110 D112:D117 D119:D121 D123:D139 F29:F32 F66:F72 F74:F77 F79:F83 F85:F89 F91:F99 F101:F110 F112:F117 F119:F139 H4:H10 H12:H19 H21:H27 H29:H32 H34:H40 D4:D10 F4:F10 D12:D19 F12:F19 D21:D27 F21:F27 D34:D40 F34:F40 D42:D48 F42:F48 D50:D55 F50:F55 D57:D64 F57:F64">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Block / Skip">
       <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(D4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4:D6 F4:F6 H4:H6 D8:D10 F8:F10 H8:H10 D12:D14 F12:F14 H12:H14 D16:D19 F16:F19 H16:H19 D21 F21 H21 D23:D24 F23:F24 D26:D27 F26:F27 D29:D36 F29:F36 D38:D44 F38:F44 D46:D49 F46:F49 D51:D55 F51:F55 D57:D61 F57:F61 D63:D71 F63:F71 D73:D82 F73:F82 D84:D89 F84:F89 D91:D93 F91:F93 D95:D111 F95:F111" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F123:F139 D4:D10 H4:H10 F4:F10 D12:D19 H12:H19 F12:F19 D21:D27 H21:H27 D29:D32 F29:F32 H29:H32 F21:F27 D34:D40 H34:H40 F34:F40 D42:D48 F42:F48 D50:D55 F50:F55 D57:D64 D66:D72 F66:F72 D74:D77 F74:F77 D79:D83 F79:F83 D85:D89 F85:F89 D91:D99 F91:F99 D101:D110 F101:F110 D112:D117 F112:F117 D119:D121 F119:F121 D123:D139 F57:F64" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>